<commit_message>
created notebooks for lin reg and gru
</commit_message>
<xml_diff>
--- a/NN_results/AMZN_NN_results.xlsx
+++ b/NN_results/AMZN_NN_results.xlsx
@@ -451,7 +451,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2361.26708984375</v>
+        <v>2371.200439453125</v>
       </c>
       <c r="C2" t="n">
         <v>2409</v>
@@ -462,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2380.817138671875</v>
+        <v>2391.159912109375</v>
       </c>
       <c r="C3" t="n">
         <v>2356.949951171875</v>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2372.716552734375</v>
+        <v>2379.166259765625</v>
       </c>
       <c r="C4" t="n">
         <v>2367.919921875</v>
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2365.983154296875</v>
+        <v>2374.047607421875</v>
       </c>
       <c r="C5" t="n">
         <v>2388.85009765625</v>
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2371.24462890625</v>
+        <v>2381.680419921875</v>
       </c>
       <c r="C6" t="n">
         <v>2409.780029296875</v>
@@ -506,7 +506,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2385.27001953125</v>
+        <v>2396.42724609375</v>
       </c>
       <c r="C7" t="n">
         <v>2426.260009765625</v>
@@ -517,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2401.417724609375</v>
+        <v>2412.0927734375</v>
       </c>
       <c r="C8" t="n">
         <v>2449.330078125</v>
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2419.80615234375</v>
+        <v>2430.40771484375</v>
       </c>
       <c r="C9" t="n">
         <v>2497.93994140625</v>
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2449.35546875</v>
+        <v>2461.4736328125</v>
       </c>
       <c r="C10" t="n">
         <v>2446.739990234375</v>
@@ -550,7 +550,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2449.474853515625</v>
+        <v>2456.62109375</v>
       </c>
       <c r="C11" t="n">
         <v>2436.8798828125</v>
@@ -561,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2438.89599609375</v>
+        <v>2445.56396484375</v>
       </c>
       <c r="C12" t="n">
         <v>2421.860107421875</v>
@@ -572,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>2425.202880859375</v>
+        <v>2432.737548828125</v>
       </c>
       <c r="C13" t="n">
         <v>2410.389892578125</v>
@@ -583,7 +583,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2412.56591796875</v>
+        <v>2420.9404296875</v>
       </c>
       <c r="C14" t="n">
         <v>2401.10009765625</v>
@@ -594,7 +594,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2402.08544921875</v>
+        <v>2410.858154296875</v>
       </c>
       <c r="C15" t="n">
         <v>2442.3701171875</v>
@@ -605,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2412.372802734375</v>
+        <v>2423.982177734375</v>
       </c>
       <c r="C16" t="n">
         <v>2471.0400390625</v>
@@ -616,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2433.94970703125</v>
+        <v>2446.057373046875</v>
       </c>
       <c r="C17" t="n">
         <v>2472.409912109375</v>
@@ -627,7 +627,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2448.898681640625</v>
+        <v>2458.948974609375</v>
       </c>
       <c r="C18" t="n">
         <v>2478.39990234375</v>
@@ -638,7 +638,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2457.941162109375</v>
+        <v>2467.070068359375</v>
       </c>
       <c r="C19" t="n">
         <v>2460.60009765625</v>
@@ -649,7 +649,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>2455.240966796875</v>
+        <v>2463.0078125</v>
       </c>
       <c r="C20" t="n">
         <v>2483</v>
@@ -660,7 +660,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2459.5390625</v>
+        <v>2469.313232421875</v>
       </c>
       <c r="C21" t="n">
         <v>2524.06005859375</v>
@@ -671,7 +671,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>2479.404052734375</v>
+        <v>2491.7373046875</v>
       </c>
       <c r="C22" t="n">
         <v>2600.860107421875</v>
@@ -682,7 +682,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>2522.897216796875</v>
+        <v>2538.260498046875</v>
       </c>
       <c r="C23" t="n">
         <v>2647.449951171875</v>
@@ -693,7 +693,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>2569.83740234375</v>
+        <v>2584.6142578125</v>
       </c>
       <c r="C24" t="n">
         <v>2557.9599609375</v>
@@ -704,7 +704,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>2565.427978515625</v>
+        <v>2570.0859375</v>
       </c>
       <c r="C25" t="n">
         <v>2545.02001953125</v>
@@ -715,7 +715,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2545.96728515625</v>
+        <v>2550.01171875</v>
       </c>
       <c r="C26" t="n">
         <v>2572.679931640625</v>
@@ -726,7 +726,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2541.86279296875</v>
+        <v>2551.259033203125</v>
       </c>
       <c r="C27" t="n">
         <v>2615.27001953125</v>
@@ -737,7 +737,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>2559.276611328125</v>
+        <v>2572.7626953125</v>
       </c>
       <c r="C28" t="n">
         <v>2640.97998046875</v>
@@ -748,7 +748,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>2583.558837890625</v>
+        <v>2596.9296875</v>
       </c>
       <c r="C29" t="n">
         <v>2653.97998046875</v>
@@ -759,7 +759,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>2603.440673828125</v>
+        <v>2614.922607421875</v>
       </c>
       <c r="C30" t="n">
         <v>2675.010009765625</v>
@@ -770,7 +770,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>2621.201171875</v>
+        <v>2632.214599609375</v>
       </c>
       <c r="C31" t="n">
         <v>2713.820068359375</v>
@@ -781,7 +781,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>2644.676513671875</v>
+        <v>2657.255615234375</v>
       </c>
       <c r="C32" t="n">
         <v>2764.409912109375</v>
@@ -792,7 +792,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>2677.270751953125</v>
+        <v>2691.930419921875</v>
       </c>
       <c r="C33" t="n">
         <v>2734.39990234375</v>
@@ -803,7 +803,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>2688.64453125</v>
+        <v>2698.268310546875</v>
       </c>
       <c r="C34" t="n">
         <v>2754.580078125</v>
@@ -814,7 +814,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>2696.908203125</v>
+        <v>2706.49755859375</v>
       </c>
       <c r="C35" t="n">
         <v>2692.8701171875</v>
@@ -825,7 +825,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>2681.154052734375</v>
+        <v>2685.690673828125</v>
       </c>
       <c r="C36" t="n">
         <v>2680.3798828125</v>
@@ -836,7 +836,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>2661.5751953125</v>
+        <v>2666.5078125</v>
       </c>
       <c r="C37" t="n">
         <v>2758.820068359375</v>
@@ -847,7 +847,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>2675.94677734375</v>
+        <v>2689.57080078125</v>
       </c>
       <c r="C38" t="n">
         <v>2878.699951171875</v>
@@ -858,7 +858,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>2733.219970703125</v>
+        <v>2755.28515625</v>
       </c>
       <c r="C39" t="n">
         <v>2890.300048828125</v>
@@ -869,7 +869,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>2779.95849609375</v>
+        <v>2797.542236328125</v>
       </c>
       <c r="C40" t="n">
         <v>3057.0400390625</v>
@@ -880,7 +880,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>2856.393310546875</v>
+        <v>2881.5615234375</v>
       </c>
       <c r="C41" t="n">
         <v>3000.1201171875</v>
@@ -891,7 +891,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>2891.772705078125</v>
+        <v>2906.056396484375</v>
       </c>
       <c r="C42" t="n">
         <v>3081.110107421875</v>
@@ -902,7 +902,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>2926.76806640625</v>
+        <v>2942.61376953125</v>
       </c>
       <c r="C43" t="n">
         <v>3182.6298828125</v>
@@ -913,7 +913,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>2977.749267578125</v>
+        <v>3000.808349609375</v>
       </c>
       <c r="C44" t="n">
         <v>3200</v>
@@ -924,7 +924,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>3018.23974609375</v>
+        <v>3038.533447265625</v>
       </c>
       <c r="C45" t="n">
         <v>3104</v>
@@ -935,7 +935,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>3015.399169921875</v>
+        <v>3019.465087890625</v>
       </c>
       <c r="C46" t="n">
         <v>3084</v>
@@ -946,7 +946,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>2996.935546875</v>
+        <v>2996.0830078125</v>
       </c>
       <c r="C47" t="n">
         <v>3008.8701171875</v>
@@ -957,7 +957,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>2961.421630859375</v>
+        <v>2955.967529296875</v>
       </c>
       <c r="C48" t="n">
         <v>2999.89990234375</v>
@@ -968,7 +968,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>2931.93115234375</v>
+        <v>2930.42138671875</v>
       </c>
       <c r="C49" t="n">
         <v>2961.969970703125</v>
@@ -979,7 +979,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>2904.720458984375</v>
+        <v>2904.734375</v>
       </c>
       <c r="C50" t="n">
         <v>3196.840087890625</v>
@@ -990,7 +990,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>2955.830810546875</v>
+        <v>2981.215087890625</v>
       </c>
       <c r="C51" t="n">
         <v>3138.2900390625</v>
@@ -1001,7 +1001,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>2990.489013671875</v>
+        <v>3008.62109375</v>
       </c>
       <c r="C52" t="n">
         <v>3099.909912109375</v>
@@ -1012,7 +1012,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>2995.74755859375</v>
+        <v>3001.85302734375</v>
       </c>
       <c r="C53" t="n">
         <v>2986.550048828125</v>
@@ -1023,7 +1023,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>2960.20068359375</v>
+        <v>2951.943115234375</v>
       </c>
       <c r="C54" t="n">
         <v>3008.909912109375</v>
@@ -1034,7 +1034,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>2932.629150390625</v>
+        <v>2930.454345703125</v>
       </c>
       <c r="C55" t="n">
         <v>3055.2099609375</v>
@@ -1045,7 +1045,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>2931.95751953125</v>
+        <v>2941.08203125</v>
       </c>
       <c r="C56" t="n">
         <v>3000.330078125</v>
@@ -1056,7 +1056,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>2923.37109375</v>
+        <v>2929.015625</v>
       </c>
       <c r="C57" t="n">
         <v>3033.530029296875</v>
@@ -1067,7 +1067,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>2924.604736328125</v>
+        <v>2932.724609375</v>
       </c>
       <c r="C58" t="n">
         <v>3051.8798828125</v>
@@ -1078,7 +1078,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>2933.202392578125</v>
+        <v>2943.490234375</v>
       </c>
       <c r="C59" t="n">
         <v>3164.679931640625</v>
@@ -1089,7 +1089,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>2972.103271484375</v>
+        <v>2992.2265625</v>
       </c>
       <c r="C60" t="n">
         <v>3111.889892578125</v>
@@ -1100,7 +1100,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>2989.060791015625</v>
+        <v>3000.890380859375</v>
       </c>
       <c r="C61" t="n">
         <v>3138.830078125</v>
@@ -1111,7 +1111,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>3000.721923828125</v>
+        <v>3010.49951171875</v>
       </c>
       <c r="C62" t="n">
         <v>3205.030029296875</v>
@@ -1122,7 +1122,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>3024.857177734375</v>
+        <v>3040.088623046875</v>
       </c>
       <c r="C63" t="n">
         <v>3225</v>
@@ -1133,7 +1133,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>3048.914794921875</v>
+        <v>3064.4287109375</v>
       </c>
       <c r="C64" t="n">
         <v>3167.4599609375</v>
@@ -1144,7 +1144,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>3049.06103515625</v>
+        <v>3054.822509765625</v>
       </c>
       <c r="C65" t="n">
         <v>3148.159912109375</v>
@@ -1155,7 +1155,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>3037.656005859375</v>
+        <v>3039.07958984375</v>
       </c>
       <c r="C66" t="n">
         <v>3080.669921875</v>
@@ -1166,7 +1166,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>3009.856201171875</v>
+        <v>3005.732177734375</v>
       </c>
       <c r="C67" t="n">
         <v>3162.239990234375</v>
@@ -1177,7 +1177,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>3009.62353515625</v>
+        <v>3017.37744140625</v>
       </c>
       <c r="C68" t="n">
         <v>3161.02001953125</v>
@@ -1188,7 +1188,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>3017.434814453125</v>
+        <v>3028.071044921875</v>
       </c>
       <c r="C69" t="n">
         <v>3148.02001953125</v>
@@ -1199,7 +1199,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>3020.495849609375</v>
+        <v>3028.199462890625</v>
       </c>
       <c r="C70" t="n">
         <v>3182.409912109375</v>
@@ -1210,7 +1210,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>3029.913818359375</v>
+        <v>3039.636474609375</v>
       </c>
       <c r="C71" t="n">
         <v>3312.489990234375</v>
@@ -1221,7 +1221,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>3071.71826171875</v>
+        <v>3093.9658203125</v>
       </c>
       <c r="C72" t="n">
         <v>3260.47998046875</v>
@@ -1232,7 +1232,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>3092.986328125</v>
+        <v>3106.787109375</v>
       </c>
       <c r="C73" t="n">
         <v>3297.3701171875</v>
@@ -1243,7 +1243,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>3109.795166015625</v>
+        <v>3121.4091796875</v>
       </c>
       <c r="C74" t="n">
         <v>3284.719970703125</v>
@@ -1254,7 +1254,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>3116.638916015625</v>
+        <v>3124.5771484375</v>
       </c>
       <c r="C75" t="n">
         <v>3307.4599609375</v>
@@ -1265,7 +1265,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>3124.24462890625</v>
+        <v>3133.0390625</v>
       </c>
       <c r="C76" t="n">
         <v>3346.489990234375</v>
@@ -1276,7 +1276,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>3139.32177734375</v>
+        <v>3151.689208984375</v>
       </c>
       <c r="C77" t="n">
         <v>3441.85009765625</v>
@@ -1287,7 +1287,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>3174.111328125</v>
+        <v>3195.1484375</v>
       </c>
       <c r="C78" t="n">
         <v>3400</v>
@@ -1298,7 +1298,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>3191.893310546875</v>
+        <v>3204.716064453125</v>
       </c>
       <c r="C79" t="n">
         <v>3401.800048828125</v>
@@ -1309,7 +1309,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>3198.978271484375</v>
+        <v>3206.13525390625</v>
       </c>
       <c r="C80" t="n">
         <v>3450.9599609375</v>
@@ -1320,7 +1320,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>3212.283935546875</v>
+        <v>3222.922607421875</v>
       </c>
       <c r="C81" t="n">
         <v>3499.1201171875</v>
@@ -1331,7 +1331,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>3234.06591796875</v>
+        <v>3249.3115234375</v>
       </c>
       <c r="C82" t="n">
         <v>3531.449951171875</v>
@@ -1342,7 +1342,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>3257.860107421875</v>
+        <v>3273.98828125</v>
       </c>
       <c r="C83" t="n">
         <v>3368</v>
@@ -1353,7 +1353,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>3238.292724609375</v>
+        <v>3230.9365234375</v>
       </c>
       <c r="C84" t="n">
         <v>3294.6201171875</v>
@@ -1364,7 +1364,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>3195.72802734375</v>
+        <v>3176.452880859375</v>
       </c>
       <c r="C85" t="n">
         <v>3149.840087890625</v>
@@ -1375,7 +1375,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>3126.617431640625</v>
+        <v>3096.86181640625</v>
       </c>
       <c r="C86" t="n">
         <v>3268.610107421875</v>
@@ -1386,7 +1386,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>3101.63720703125</v>
+        <v>3096.677734375</v>
       </c>
       <c r="C87" t="n">
         <v>3175.110107421875</v>
@@ -1397,7 +1397,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>3076.214599609375</v>
+        <v>3072.298583984375</v>
       </c>
       <c r="C88" t="n">
         <v>3116.219970703125</v>
@@ -1408,7 +1408,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>3042.97705078125</v>
+        <v>3035.1083984375</v>
       </c>
       <c r="C89" t="n">
         <v>3102.969970703125</v>
@@ -1419,7 +1419,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>3014.9189453125</v>
+        <v>3009.891357421875</v>
       </c>
       <c r="C90" t="n">
         <v>3156.1298828125</v>
@@ -1430,7 +1430,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>3012.5263671875</v>
+        <v>3018.49951171875</v>
       </c>
       <c r="C91" t="n">
         <v>3078.10009765625</v>
@@ -1441,7 +1441,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>2996.828857421875</v>
+        <v>2997.53759765625</v>
       </c>
       <c r="C92" t="n">
         <v>3008.72998046875</v>
@@ -1452,7 +1452,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>2963.173828125</v>
+        <v>2957.09228515625</v>
       </c>
       <c r="C93" t="n">
         <v>2954.909912109375</v>
@@ -1463,7 +1463,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>2921.227294921875</v>
+        <v>2913.78173828125</v>
       </c>
       <c r="C94" t="n">
         <v>2960.469970703125</v>
@@ -1474,7 +1474,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>2893.99755859375</v>
+        <v>2893.766357421875</v>
       </c>
       <c r="C95" t="n">
         <v>3128.989990234375</v>
@@ -1485,7 +1485,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>2930.3857421875</v>
+        <v>2951.16259765625</v>
       </c>
       <c r="C96" t="n">
         <v>2999.860107421875</v>
@@ -1496,7 +1496,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>2931.850341796875</v>
+        <v>2939.138671875</v>
       </c>
       <c r="C97" t="n">
         <v>3019.7900390625</v>
@@ -1507,7 +1507,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>2927.710205078125</v>
+        <v>2932.25927734375</v>
       </c>
       <c r="C98" t="n">
         <v>3095.1298828125</v>
@@ -1518,7 +1518,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>2945.391845703125</v>
+        <v>2958.405517578125</v>
       </c>
       <c r="C99" t="n">
         <v>3174.050048828125</v>
@@ -1529,7 +1529,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>2984.459716796875</v>
+        <v>3004.96337890625</v>
       </c>
       <c r="C100" t="n">
         <v>3144.8798828125</v>
@@ -1540,7 +1540,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>3005.722900390625</v>
+        <v>3019.2607421875</v>
       </c>
       <c r="C101" t="n">
         <v>3148.72998046875</v>
@@ -1551,7 +1551,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>3015.056640625</v>
+        <v>3023.9931640625</v>
       </c>
       <c r="C102" t="n">
         <v>3221.260009765625</v>
@@ -1562,7 +1562,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>3037.441650390625</v>
+        <v>3052.151611328125</v>
       </c>
       <c r="C103" t="n">
         <v>3125</v>
@@ -1573,7 +1573,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>3030.23779296875</v>
+        <v>3033.630126953125</v>
       </c>
       <c r="C104" t="n">
         <v>3199.199951171875</v>
@@ -1584,7 +1584,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>3037.00390625</v>
+        <v>3046.22216796875</v>
       </c>
       <c r="C105" t="n">
         <v>3099.9599609375</v>
@@ -1595,7 +1595,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>3019.751708984375</v>
+        <v>3019.790283203125</v>
       </c>
       <c r="C106" t="n">
         <v>3195.68994140625</v>
@@ -1606,7 +1606,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>3027.310302734375</v>
+        <v>3037.3212890625</v>
       </c>
       <c r="C107" t="n">
         <v>3190.550048828125</v>
@@ -1617,7 +1617,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>3038.180419921875</v>
+        <v>3049.423828125</v>
       </c>
       <c r="C108" t="n">
         <v>3286.64990234375</v>
@@ -1628,7 +1628,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>3070.614501953125</v>
+        <v>3089.514404296875</v>
       </c>
       <c r="C109" t="n">
         <v>3442.929931640625</v>
@@ -1639,7 +1639,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>3135.812744140625</v>
+        <v>3167.550048828125</v>
       </c>
       <c r="C110" t="n">
         <v>3443.6298828125</v>
@@ -1650,7 +1650,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>3184.42041015625</v>
+        <v>3209.63134765625</v>
       </c>
       <c r="C111" t="n">
         <v>3363.7099609375</v>
@@ -1661,7 +1661,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>3192.3671875</v>
+        <v>3198.680419921875</v>
       </c>
       <c r="C112" t="n">
         <v>3338.64990234375</v>
@@ -1672,7 +1672,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>3181.040771484375</v>
+        <v>3178.862060546875</v>
       </c>
       <c r="C113" t="n">
         <v>3272.7099609375</v>
@@ -1683,7 +1683,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>3153.6181640625</v>
+        <v>3145.406005859375</v>
       </c>
       <c r="C114" t="n">
         <v>3207.2099609375</v>
@@ -1694,7 +1694,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>3115.6005859375</v>
+        <v>3103.967529296875</v>
       </c>
       <c r="C115" t="n">
         <v>3217.010009765625</v>
@@ -1705,7 +1705,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>3090.27978515625</v>
+        <v>3085.87353515625</v>
       </c>
       <c r="C116" t="n">
         <v>3184.93994140625</v>
@@ -1716,7 +1716,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>3069.781005859375</v>
+        <v>3067.975830078125</v>
       </c>
       <c r="C117" t="n">
         <v>3176.39990234375</v>
@@ -1727,7 +1727,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>3055.26611328125</v>
+        <v>3055.73779296875</v>
       </c>
       <c r="C118" t="n">
         <v>3204.39990234375</v>
@@ -1738,7 +1738,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>3054.510009765625</v>
+        <v>3060.418701171875</v>
       </c>
       <c r="C119" t="n">
         <v>3207.0400390625</v>
@@ -1749,7 +1749,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>3058.1796875</v>
+        <v>3065.582763671875</v>
       </c>
       <c r="C120" t="n">
         <v>3286.330078125</v>
@@ -1760,7 +1760,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>3081.662841796875</v>
+        <v>3096.7421875</v>
       </c>
       <c r="C121" t="n">
         <v>3162.780029296875</v>
@@ -1771,7 +1771,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>3070.188720703125</v>
+        <v>3070.402099609375</v>
       </c>
       <c r="C122" t="n">
         <v>3211.010009765625</v>
@@ -1782,7 +1782,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>3064.885986328125</v>
+        <v>3068.05078125</v>
       </c>
       <c r="C123" t="n">
         <v>3036.14990234375</v>
@@ -1793,7 +1793,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>3018.4814453125</v>
+        <v>3005.58203125</v>
       </c>
       <c r="C124" t="n">
         <v>3004.47998046875</v>
@@ -1804,7 +1804,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>2967.281494140625</v>
+        <v>2954.78759765625</v>
       </c>
       <c r="C125" t="n">
         <v>3048.409912109375</v>
@@ -1815,7 +1815,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>2946.05419921875</v>
+        <v>2947.51416015625</v>
       </c>
       <c r="C126" t="n">
         <v>3241.159912109375</v>
@@ -1826,7 +1826,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>2995.550048828125</v>
+        <v>3021.312744140625</v>
       </c>
       <c r="C127" t="n">
         <v>3322</v>
@@ -1837,7 +1837,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>3064.68310546875</v>
+        <v>3095.593017578125</v>
       </c>
       <c r="C128" t="n">
         <v>3311.3701171875</v>
@@ -1848,7 +1848,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>3107.537353515625</v>
+        <v>3127.509521484375</v>
       </c>
       <c r="C129" t="n">
         <v>3143.739990234375</v>
@@ -1859,7 +1859,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>3085.705078125</v>
+        <v>3078.369873046875</v>
       </c>
       <c r="C130" t="n">
         <v>3035.02001953125</v>
@@ -1870,7 +1870,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>3025.637451171875</v>
+        <v>3004.462646484375</v>
       </c>
       <c r="C131" t="n">
         <v>3137.389892578125</v>
@@ -1881,7 +1881,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>3003.37451171875</v>
+        <v>3002.921142578125</v>
       </c>
       <c r="C132" t="n">
         <v>3110.280029296875</v>
@@ -1892,7 +1892,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>2994.7431640625</v>
+        <v>3000.944091796875</v>
       </c>
       <c r="C133" t="n">
         <v>3128.81005859375</v>
@@ -1903,7 +1903,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>2997.398193359375</v>
+        <v>3006.306396484375</v>
       </c>
       <c r="C134" t="n">
         <v>3131.06005859375</v>
@@ -1914,7 +1914,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>3002.088623046875</v>
+        <v>3010.4482421875</v>
       </c>
       <c r="C135" t="n">
         <v>3135.659912109375</v>
@@ -1925,7 +1925,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>3006.32470703125</v>
+        <v>3014.021728515625</v>
       </c>
       <c r="C136" t="n">
         <v>3105.4599609375</v>
@@ -1936,7 +1936,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>3000.520263671875</v>
+        <v>3004.498291015625</v>
       </c>
       <c r="C137" t="n">
         <v>3117.02001953125</v>
@@ -1947,7 +1947,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>2997.14111328125</v>
+        <v>3002.540283203125</v>
       </c>
       <c r="C138" t="n">
         <v>3099.39990234375</v>
@@ -1958,7 +1958,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>2991.1103515625</v>
+        <v>2995.941162109375</v>
       </c>
       <c r="C139" t="n">
         <v>3098.389892578125</v>
@@ -1969,7 +1969,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>2986.2646484375</v>
+        <v>2991.68896484375</v>
       </c>
       <c r="C140" t="n">
         <v>3118.06005859375</v>
@@ -1980,7 +1980,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>2988.94677734375</v>
+        <v>2997.198974609375</v>
       </c>
       <c r="C141" t="n">
         <v>3185.070068359375</v>
@@ -1991,7 +1991,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>3010.88330078125</v>
+        <v>3025.963134765625</v>
       </c>
       <c r="C142" t="n">
         <v>3195.340087890625</v>
@@ -2002,7 +2002,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>3032.282958984375</v>
+        <v>3046.574951171875</v>
       </c>
       <c r="C143" t="n">
         <v>3168.0400390625</v>
@@ -2013,7 +2013,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>3037.994873046875</v>
+        <v>3045.714599609375</v>
       </c>
       <c r="C144" t="n">
         <v>3220.080078125</v>
@@ -2024,7 +2024,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>3050.9892578125</v>
+        <v>3061.906982421875</v>
       </c>
       <c r="C145" t="n">
         <v>3203.530029296875</v>
@@ -2035,7 +2035,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>3057.355712890625</v>
+        <v>3066.060302734375</v>
       </c>
       <c r="C146" t="n">
         <v>3186.72998046875</v>
@@ -2046,7 +2046,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>3055.288330078125</v>
+        <v>3060.590087890625</v>
       </c>
       <c r="C147" t="n">
         <v>3162.580078125</v>
@@ -2057,7 +2057,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>3045.549560546875</v>
+        <v>3047.9765625</v>
       </c>
       <c r="C148" t="n">
         <v>3158</v>
@@ -2068,7 +2068,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>3036.208740234375</v>
+        <v>3039.258544921875</v>
       </c>
       <c r="C149" t="n">
         <v>3177.2900390625</v>
@@ -2079,7 +2079,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>3035.688720703125</v>
+        <v>3042.51806640625</v>
       </c>
       <c r="C150" t="n">
         <v>3104.199951171875</v>
@@ -2090,7 +2090,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>3018.525390625</v>
+        <v>3018.511962890625</v>
       </c>
       <c r="C151" t="n">
         <v>3101.489990234375</v>
@@ -2101,7 +2101,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>3001.796875</v>
+        <v>3002.178466796875</v>
       </c>
       <c r="C152" t="n">
         <v>3116.419921875</v>
@@ -2112,7 +2112,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>2995.572021484375</v>
+        <v>3000.603515625</v>
       </c>
       <c r="C153" t="n">
         <v>3156.969970703125</v>
@@ -2123,7 +2123,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>3005.580810546875</v>
+        <v>3016.6083984375</v>
       </c>
       <c r="C154" t="n">
         <v>3165.1201171875</v>
@@ -2134,7 +2134,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>3018.16259765625</v>
+        <v>3029.46435546875</v>
       </c>
       <c r="C155" t="n">
         <v>3240.9599609375</v>
@@ -2145,7 +2145,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>3046.435791015625</v>
+        <v>3063.1484375</v>
       </c>
       <c r="C156" t="n">
         <v>3236.080078125</v>
@@ -2156,7 +2156,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>3066.90234375</v>
+        <v>3080.370849609375</v>
       </c>
       <c r="C157" t="n">
         <v>3201.64990234375</v>
@@ -2167,7 +2167,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>3068.70458984375</v>
+        <v>3074.485107421875</v>
       </c>
       <c r="C158" t="n">
         <v>3206.179931640625</v>
@@ -2178,7 +2178,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>3066.078369140625</v>
+        <v>3070.65869140625</v>
       </c>
       <c r="C159" t="n">
         <v>3206.52001953125</v>
@@ -2189,7 +2189,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>3063.8076171875</v>
+        <v>3069.333251953125</v>
       </c>
       <c r="C160" t="n">
         <v>3185.27001953125</v>
@@ -2200,7 +2200,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>3057.280029296875</v>
+        <v>3061.26904296875</v>
       </c>
       <c r="C161" t="n">
         <v>3172.68994140625</v>
@@ -2211,7 +2211,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>3048.699951171875</v>
+        <v>3051.843017578125</v>
       </c>
       <c r="C162" t="n">
         <v>3283.9599609375</v>
@@ -2222,7 +2222,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>3071.630615234375</v>
+        <v>3087.46484375</v>
       </c>
       <c r="C163" t="n">
         <v>3322</v>
@@ -2233,7 +2233,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>3104.368896484375</v>
+        <v>3123.734130859375</v>
       </c>
       <c r="C164" t="n">
         <v>3285.85009765625</v>
@@ -2244,7 +2244,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>3118.07666015625</v>
+        <v>3128.5439453125</v>
       </c>
       <c r="C165" t="n">
         <v>3256.929931640625</v>
@@ -2255,7 +2255,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>3114.345703125</v>
+        <v>3117.028564453125</v>
       </c>
       <c r="C166" t="n">
         <v>3186.6298828125</v>
@@ -2266,7 +2266,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>3089.953369140625</v>
+        <v>3084.406494140625</v>
       </c>
       <c r="C167" t="n">
         <v>3218.510009765625</v>
@@ -2277,7 +2277,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>3076.605712890625</v>
+        <v>3077.364013671875</v>
       </c>
       <c r="C168" t="n">
         <v>3138.3798828125</v>
@@ -2288,7 +2288,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>3051.3193359375</v>
+        <v>3047.77978515625</v>
       </c>
       <c r="C169" t="n">
         <v>3162.159912109375</v>
@@ -2299,7 +2299,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>3037.471435546875</v>
+        <v>3038.902099609375</v>
       </c>
       <c r="C170" t="n">
         <v>3182.699951171875</v>
@@ -2310,7 +2310,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>3037.45703125</v>
+        <v>3044.494873046875</v>
       </c>
       <c r="C171" t="n">
         <v>3114.2099609375</v>
@@ -2321,7 +2321,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>3022.865966796875</v>
+        <v>3023.56298828125</v>
       </c>
       <c r="C172" t="n">
         <v>3120.830078125</v>
@@ -2332,7 +2332,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>3010.63232421875</v>
+        <v>3012.291259765625</v>
       </c>
       <c r="C173" t="n">
         <v>3165.889892578125</v>
@@ -2343,7 +2343,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>3015.754150390625</v>
+        <v>3024.621826171875</v>
       </c>
       <c r="C174" t="n">
         <v>3127.469970703125</v>
@@ -2354,7 +2354,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>3013.417236328125</v>
+        <v>3019.225341796875</v>
       </c>
       <c r="C175" t="n">
         <v>3104.25</v>
@@ -2365,7 +2365,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>3003.154541015625</v>
+        <v>3005.65771484375</v>
       </c>
       <c r="C176" t="n">
         <v>3120.760009765625</v>
@@ -2376,7 +2376,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>2998.87890625</v>
+        <v>3004.12451171875</v>
       </c>
       <c r="C177" t="n">
         <v>3263.3798828125</v>
@@ -2387,7 +2387,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>3036.406005859375</v>
+        <v>3057.444580078125</v>
       </c>
       <c r="C178" t="n">
         <v>3306.989990234375</v>
@@ -2398,7 +2398,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>3081.923095703125</v>
+        <v>3105.4892578125</v>
       </c>
       <c r="C179" t="n">
         <v>3292.22998046875</v>
@@ -2409,7 +2409,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>3107.9072265625</v>
+        <v>3122.879638671875</v>
       </c>
       <c r="C180" t="n">
         <v>3294</v>
@@ -2420,7 +2420,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>3119.578125</v>
+        <v>3128.646484375</v>
       </c>
       <c r="C181" t="n">
         <v>3326.1298828125</v>
@@ -2431,7 +2431,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>3131.578369140625</v>
+        <v>3141.823974609375</v>
       </c>
       <c r="C182" t="n">
         <v>3232.580078125</v>
@@ -2442,7 +2442,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>3117.214599609375</v>
+        <v>3116.2041015625</v>
       </c>
       <c r="C183" t="n">
         <v>3237.6201171875</v>
@@ -2453,7 +2453,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>3101.72900390625</v>
+        <v>3100.758056640625</v>
       </c>
       <c r="C184" t="n">
         <v>3206.199951171875</v>
@@ -2464,7 +2464,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>3084.1845703125</v>
+        <v>3083.16748046875</v>
       </c>
       <c r="C185" t="n">
         <v>3342.8798828125</v>
@@ -2475,7 +2475,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>3106.950439453125</v>
+        <v>3123.17919921875</v>
       </c>
       <c r="C186" t="n">
         <v>3380</v>
@@ -2486,7 +2486,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>3141.6708984375</v>
+        <v>3162.355224609375</v>
       </c>
       <c r="C187" t="n">
         <v>3312.530029296875</v>
@@ -2497,7 +2497,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>3149.8212890625</v>
+        <v>3157.50927734375</v>
       </c>
       <c r="C188" t="n">
         <v>3331</v>
@@ -2508,7 +2508,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>3151.85693359375</v>
+        <v>3156.5517578125</v>
       </c>
       <c r="C189" t="n">
         <v>3352.14990234375</v>
@@ -2519,7 +2519,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>3157.087646484375</v>
+        <v>3164.2646484375</v>
       </c>
       <c r="C190" t="n">
         <v>3322.93994140625</v>
@@ -2530,7 +2530,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>3154.81787109375</v>
+        <v>3158.946533203125</v>
       </c>
       <c r="C191" t="n">
         <v>3305</v>
@@ -2541,7 +2541,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>3146.97119140625</v>
+        <v>3148.47021484375</v>
       </c>
       <c r="C192" t="n">
         <v>3286.580078125</v>
@@ -2552,7 +2552,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>3135.98974609375</v>
+        <v>3136.243408203125</v>
       </c>
       <c r="C193" t="n">
         <v>3262.1298828125</v>
@@ -2563,7 +2563,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>3122.111572265625</v>
+        <v>3121.34326171875</v>
       </c>
       <c r="C194" t="n">
         <v>3277.7099609375</v>
@@ -2574,7 +2574,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>3116.130859375</v>
+        <v>3119.186279296875</v>
       </c>
       <c r="C195" t="n">
         <v>3268.949951171875</v>
@@ -2585,7 +2585,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>3112.391845703125</v>
+        <v>3116.460693359375</v>
       </c>
       <c r="C196" t="n">
         <v>3308.639892578125</v>
@@ -2596,7 +2596,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>3120.1875</v>
+        <v>3129.066162109375</v>
       </c>
       <c r="C197" t="n">
         <v>3328.22998046875</v>
@@ -2607,7 +2607,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>3133.072021484375</v>
+        <v>3143.921875</v>
       </c>
       <c r="C198" t="n">
         <v>3249.89990234375</v>
@@ -2618,7 +2618,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>3123.357177734375</v>
+        <v>3123.68115234375</v>
       </c>
       <c r="C199" t="n">
         <v>3180.739990234375</v>
@@ -2629,7 +2629,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>3093.242919921875</v>
+        <v>3084.681396484375</v>
       </c>
       <c r="C200" t="n">
         <v>3194.5</v>
@@ -2640,7 +2640,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>3071.370361328125</v>
+        <v>3068.151123046875</v>
       </c>
       <c r="C201" t="n">
         <v>3159.530029296875</v>
@@ -2651,7 +2651,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>3051.227783203125</v>
+        <v>3049.930419921875</v>
       </c>
       <c r="C202" t="n">
         <v>3057.159912109375</v>
@@ -2662,7 +2662,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>3011.6005859375</v>
+        <v>3002.52294921875</v>
       </c>
       <c r="C203" t="n">
         <v>3092.929931640625</v>
@@ -2673,7 +2673,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>2989.526611328125</v>
+        <v>2988.461669921875</v>
       </c>
       <c r="C204" t="n">
         <v>3146.139892578125</v>
@@ -2684,7 +2684,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>2995.412841796875</v>
+        <v>3005.392333984375</v>
       </c>
       <c r="C205" t="n">
         <v>3094.530029296875</v>
@@ -2695,7 +2695,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>2992.223876953125</v>
+        <v>2997.91259765625</v>
       </c>
       <c r="C206" t="n">
         <v>3005</v>
@@ -2706,7 +2706,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>2962.2158203125</v>
+        <v>2957.274658203125</v>
       </c>
       <c r="C207" t="n">
         <v>2977.570068359375</v>
@@ -2717,7 +2717,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>2927.5185546875</v>
+        <v>2922.39013671875</v>
       </c>
       <c r="C208" t="n">
         <v>3000.4599609375</v>
@@ -2728,7 +2728,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>2911.24951171875</v>
+        <v>2914.48583984375</v>
       </c>
       <c r="C209" t="n">
         <v>2951.949951171875</v>
@@ -2739,7 +2739,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>2892.320068359375</v>
+        <v>2894.8916015625</v>
       </c>
       <c r="C210" t="n">
         <v>3062.85009765625</v>
@@ -2750,7 +2750,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>2911.5888671875</v>
+        <v>2926.192138671875</v>
       </c>
       <c r="C211" t="n">
         <v>3057.639892578125</v>
@@ -2761,7 +2761,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>2931.821533203125</v>
+        <v>2945.66748046875</v>
       </c>
       <c r="C212" t="n">
         <v>3113.590087890625</v>
@@ -2772,7 +2772,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>2959.4833984375</v>
+        <v>2974.9287109375</v>
       </c>
       <c r="C213" t="n">
         <v>3089.489990234375</v>
@@ -2783,7 +2783,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>2971.57421875</v>
+        <v>2981.526611328125</v>
       </c>
       <c r="C214" t="n">
         <v>3081.679931640625</v>
@@ -2794,7 +2794,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>2972.769287109375</v>
+        <v>2979.294677734375</v>
       </c>
       <c r="C215" t="n">
         <v>3091.860107421875</v>
@@ -2805,7 +2805,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>2973.785400390625</v>
+        <v>2981.15185546875</v>
       </c>
       <c r="C216" t="n">
         <v>3135.72998046875</v>
@@ -2816,7 +2816,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>2986.896240234375</v>
+        <v>2999.119140625</v>
       </c>
       <c r="C217" t="n">
         <v>3027.989990234375</v>
@@ -2827,7 +2827,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>2969.021484375</v>
+        <v>2969.470458984375</v>
       </c>
       <c r="C218" t="n">
         <v>3074.9599609375</v>
@@ -2838,7 +2838,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>2961.856201171875</v>
+        <v>2966.66552734375</v>
       </c>
       <c r="C219" t="n">
         <v>3110.8701171875</v>
@@ -2849,7 +2849,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>2971.02685546875</v>
+        <v>2982.2255859375</v>
       </c>
       <c r="C220" t="n">
         <v>3137.5</v>
@@ -2860,7 +2860,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>2988.444091796875</v>
+        <v>3001.979248046875</v>
       </c>
       <c r="C221" t="n">
         <v>3087.070068359375</v>
@@ -2871,7 +2871,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>2987.35302734375</v>
+        <v>2993.27197265625</v>
       </c>
       <c r="C222" t="n">
         <v>3046.260009765625</v>
@@ -2882,7 +2882,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>2970.171142578125</v>
+        <v>2970.213134765625</v>
       </c>
       <c r="C223" t="n">
         <v>3052.030029296875</v>
@@ -2893,7 +2893,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>2956.698486328125</v>
+        <v>2959.304931640625</v>
       </c>
       <c r="C224" t="n">
         <v>3075.72998046875</v>
@@ -2904,7 +2904,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>2956.359619140625</v>
+        <v>2964.383056640625</v>
       </c>
       <c r="C225" t="n">
         <v>3055.2900390625</v>
@@ -2915,7 +2915,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>2954.033203125</v>
+        <v>2960.96826171875</v>
       </c>
       <c r="C226" t="n">
         <v>3094.080078125</v>
@@ -2926,7 +2926,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>2962.52490234375</v>
+        <v>2972.793212890625</v>
       </c>
       <c r="C227" t="n">
         <v>3161</v>
@@ -2937,7 +2937,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>2989.208740234375</v>
+        <v>3005.54150390625</v>
       </c>
       <c r="C228" t="n">
         <v>3226.72998046875</v>
@@ -2948,7 +2948,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>3028.080322265625</v>
+        <v>3048.33154296875</v>
       </c>
       <c r="C229" t="n">
         <v>3223.820068359375</v>
@@ -2959,7 +2959,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>3054.24560546875</v>
+        <v>3069.378662109375</v>
       </c>
       <c r="C230" t="n">
         <v>3279.389892578125</v>
@@ -2970,7 +2970,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>3081.545166015625</v>
+        <v>3097.369384765625</v>
       </c>
       <c r="C231" t="n">
         <v>3299.300048828125</v>
@@ -2981,7 +2981,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>3104.51806640625</v>
+        <v>3119.258544921875</v>
       </c>
       <c r="C232" t="n">
         <v>3372.199951171875</v>
@@ -2992,7 +2992,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>3136.244873046875</v>
+        <v>3155.1572265625</v>
       </c>
       <c r="C233" t="n">
         <v>3379.389892578125</v>
@@ -3003,7 +3003,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>3160.870361328125</v>
+        <v>3176.916748046875</v>
       </c>
       <c r="C234" t="n">
         <v>3400</v>
@@ -3014,7 +3014,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>3179.783447265625</v>
+        <v>3193.1416015625</v>
       </c>
       <c r="C235" t="n">
         <v>3333</v>
@@ -3025,7 +3025,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>3175.219970703125</v>
+        <v>3177.446044921875</v>
       </c>
       <c r="C236" t="n">
         <v>3379.090087890625</v>
@@ -3036,7 +3036,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>3176.696044921875</v>
+        <v>3182.156982421875</v>
       </c>
       <c r="C237" t="n">
         <v>3399.43994140625</v>
@@ -3047,7 +3047,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>3184.916015625</v>
+        <v>3194.107421875</v>
       </c>
       <c r="C238" t="n">
         <v>3372.010009765625</v>
@@ -3058,7 +3058,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>3185.9296875</v>
+        <v>3191.296875</v>
       </c>
       <c r="C239" t="n">
         <v>3334.68994140625</v>
@@ -3069,7 +3069,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>3175.73583984375</v>
+        <v>3175.211181640625</v>
       </c>
       <c r="C240" t="n">
         <v>3362.02001953125</v>
@@ -3080,7 +3080,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>3172.339599609375</v>
+        <v>3175.3203125</v>
       </c>
       <c r="C241" t="n">
         <v>3309.0400390625</v>
@@ -3091,7 +3091,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>3159.884033203125</v>
+        <v>3158.86865234375</v>
       </c>
       <c r="C242" t="n">
         <v>3340.8798828125</v>
@@ -3102,7 +3102,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>3156.535888671875</v>
+        <v>3159.884521484375</v>
       </c>
       <c r="C243" t="n">
         <v>3409</v>
@@ -3113,7 +3113,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>3173.33935546875</v>
+        <v>3186.147705078125</v>
       </c>
       <c r="C244" t="n">
         <v>3417.429931640625</v>
@@ -3124,7 +3124,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>3191.5654296875</v>
+        <v>3204.67041015625</v>
       </c>
       <c r="C245" t="n">
         <v>3458.5</v>
@@ -3135,7 +3135,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>3212.730712890625</v>
+        <v>3226.7099609375</v>
       </c>
       <c r="C246" t="n">
         <v>3471.310302734375</v>
@@ -3146,7 +3146,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>3230.106201171875</v>
+        <v>3242.238525390625</v>
       </c>
       <c r="C247" t="n">
         <v>3467.420166015625</v>
@@ -3157,7 +3157,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>3239.60107421875</v>
+        <v>3247.84619140625</v>
       </c>
       <c r="C248" t="n">
         <v>3386.489990234375</v>
@@ -3168,7 +3168,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>3225.86474609375</v>
+        <v>3222.1591796875</v>
       </c>
       <c r="C249" t="n">
         <v>3311.8701171875</v>
@@ -3179,7 +3179,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>3193.1884765625</v>
+        <v>3180.218017578125</v>
       </c>
       <c r="C250" t="n">
         <v>3270.5400390625</v>
@@ -3190,7 +3190,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>3156.40673828125</v>
+        <v>3143.109375</v>
       </c>
       <c r="C251" t="n">
         <v>3306.3701171875</v>
@@ -3201,7 +3201,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>3139.91064453125</v>
+        <v>3137.97900390625</v>
       </c>
       <c r="C252" t="n">
         <v>3291.610107421875</v>
@@ -3212,7 +3212,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>3131.724609375</v>
+        <v>3133.86279296875</v>
       </c>
       <c r="C253" t="n">
         <v>3190.489990234375</v>
@@ -3223,7 +3223,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>3103.222412109375</v>
+        <v>3095.505859375</v>
       </c>
       <c r="C254" t="n">
         <v>3223.909912109375</v>
@@ -3234,7 +3234,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>3086.341552734375</v>
+        <v>3084.270751953125</v>
       </c>
       <c r="C255" t="n">
         <v>3151.93994140625</v>
@@ -3245,7 +3245,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>3060.6904296875</v>
+        <v>3055.8544921875</v>
       </c>
       <c r="C256" t="n">
         <v>3161.469970703125</v>
@@ -3256,7 +3256,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>3043.56201171875</v>
+        <v>3042.960693359375</v>
       </c>
       <c r="C257" t="n">
         <v>3222.89990234375</v>
@@ -3267,7 +3267,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>3051.110595703125</v>
+        <v>3060.837646484375</v>
       </c>
       <c r="C258" t="n">
         <v>3270.389892578125</v>
@@ -3278,7 +3278,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>3074.71142578125</v>
+        <v>3090.301513671875</v>
       </c>
       <c r="C259" t="n">
         <v>3232.280029296875</v>
@@ -3289,7 +3289,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>3083.492431640625</v>
+        <v>3092.16796875</v>
       </c>
       <c r="C260" t="n">
         <v>3231.800048828125</v>
@@ -3300,7 +3300,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>3084.443359375</v>
+        <v>3089.661865234375</v>
       </c>
       <c r="C261" t="n">
         <v>3247.679931640625</v>
@@ -3311,7 +3311,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>3087.135009765625</v>
+        <v>3093.816162109375</v>
       </c>
       <c r="C262" t="n">
         <v>3203.080078125</v>
@@ -3322,7 +3322,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>3078.359130859375</v>
+        <v>3080.644775390625</v>
       </c>
       <c r="C263" t="n">
         <v>3244.989990234375</v>
@@ -3333,7 +3333,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>3080.1826171875</v>
+        <v>3087.212646484375</v>
       </c>
       <c r="C264" t="n">
         <v>3259.050048828125</v>
@@ -3344,7 +3344,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>3088.206787109375</v>
+        <v>3097.893310546875</v>
       </c>
       <c r="C265" t="n">
         <v>3265.159912109375</v>
@@ -3355,7 +3355,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>3096.43359375</v>
+        <v>3105.743896484375</v>
       </c>
       <c r="C266" t="n">
         <v>3230.110107421875</v>
@@ -3366,7 +3366,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>3092.792724609375</v>
+        <v>3096.66552734375</v>
       </c>
       <c r="C267" t="n">
         <v>3223.070068359375</v>
@@ -3377,7 +3377,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>3085.2939453125</v>
+        <v>3087.6845703125</v>
       </c>
       <c r="C268" t="n">
         <v>3218.64990234375</v>
@@ -3388,7 +3388,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>3078.51611328125</v>
+        <v>3081.75244140625</v>
       </c>
       <c r="C269" t="n">
         <v>3233.989990234375</v>
@@ -3399,7 +3399,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>3078.430419921875</v>
+        <v>3084.73095703125</v>
       </c>
       <c r="C270" t="n">
         <v>3187.010009765625</v>
@@ -3410,7 +3410,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>3068.26416015625</v>
+        <v>3070.17138671875</v>
       </c>
       <c r="C271" t="n">
         <v>3206.219970703125</v>
@@ -3421,7 +3421,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>3063.58984375</v>
+        <v>3067.796630859375</v>
       </c>
       <c r="C272" t="n">
         <v>3198.010009765625</v>
@@ -3432,7 +3432,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>3060.185302734375</v>
+        <v>3065.1220703125</v>
       </c>
       <c r="C273" t="n">
         <v>3264.110107421875</v>
@@ -3443,7 +3443,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>3075.279296875</v>
+        <v>3087.667236328125</v>
       </c>
       <c r="C274" t="n">
         <v>3281.14990234375</v>
@@ -3454,7 +3454,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>3094.175048828125</v>
+        <v>3107.760498046875</v>
       </c>
       <c r="C275" t="n">
         <v>3349.64990234375</v>
@@ -3465,7 +3465,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="n">
-        <v>3123.8955078125</v>
+        <v>3141.557373046875</v>
       </c>
       <c r="C276" t="n">
         <v>3346.830078125</v>
@@ -3476,7 +3476,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="n">
-        <v>3144.882568359375</v>
+        <v>3158.686767578125</v>
       </c>
       <c r="C277" t="n">
         <v>3383.8701171875</v>
@@ -3487,7 +3487,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>3164.76123046875</v>
+        <v>3178.1259765625</v>
       </c>
       <c r="C278" t="n">
         <v>3383.1298828125</v>
@@ -3498,7 +3498,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="n">
-        <v>3177.420166015625</v>
+        <v>3187.816162109375</v>
       </c>
       <c r="C279" t="n">
         <v>3415.25</v>
@@ -3509,7 +3509,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="n">
-        <v>3191.390625</v>
+        <v>3202.621337890625</v>
       </c>
       <c r="C280" t="n">
         <v>3489.239990234375</v>
@@ -3520,7 +3520,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="n">
-        <v>3218.167724609375</v>
+        <v>3235.745849609375</v>
       </c>
       <c r="C281" t="n">
         <v>3486.89990234375</v>
@@ -3531,7 +3531,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="n">
-        <v>3238.714111328125</v>
+        <v>3253.172119140625</v>
       </c>
       <c r="C282" t="n">
         <v>3453.959716796875</v>
@@ -3542,7 +3542,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>3243.10888671875</v>
+        <v>3248.8154296875</v>
       </c>
       <c r="C283" t="n">
         <v>3505.43994140625</v>
@@ -3553,7 +3553,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="n">
-        <v>3253.005859375</v>
+        <v>3261.59423828125</v>
       </c>
       <c r="C284" t="n">
         <v>3503.820068359375</v>
@@ -3564,7 +3564,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="n">
-        <v>3261.31787109375</v>
+        <v>3269.456298828125</v>
       </c>
       <c r="C285" t="n">
         <v>3449.080078125</v>
@@ -3575,7 +3575,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="n">
-        <v>3254.582275390625</v>
+        <v>3254.427734375</v>
       </c>
       <c r="C286" t="n">
         <v>3401.4599609375</v>
@@ -3586,7 +3586,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="n">
-        <v>3235.2900390625</v>
+        <v>3228.324462890625</v>
       </c>
       <c r="C287" t="n">
         <v>3443.889892578125</v>
@@ -3597,7 +3597,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>3228.475830078125</v>
+        <v>3228.724853515625</v>
       </c>
       <c r="C288" t="n">
         <v>3448.139892578125</v>
@@ -3608,7 +3608,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>3229.029541015625</v>
+        <v>3233.515869140625</v>
       </c>
       <c r="C289" t="n">
         <v>3440.159912109375</v>
@@ -3619,7 +3619,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>3229.47900390625</v>
+        <v>3233.491455078125</v>
       </c>
       <c r="C290" t="n">
         <v>3432.969970703125</v>
@@ -3630,7 +3630,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>3227.834228515625</v>
+        <v>3230.396240234375</v>
       </c>
       <c r="C291" t="n">
         <v>3510.979736328125</v>
@@ -3641,7 +3641,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>3243.468505859375</v>
+        <v>3254.857421875</v>
       </c>
       <c r="C292" t="n">
         <v>3675.740234375</v>
@@ -3652,7 +3652,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="n">
-        <v>3294.35400390625</v>
+        <v>3324.014892578125</v>
       </c>
       <c r="C293" t="n">
         <v>3696.579833984375</v>
@@ -3663,7 +3663,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>3340.477294921875</v>
+        <v>3368.452392578125</v>
       </c>
       <c r="C294" t="n">
         <v>3731.41015625</v>
@@ -3674,7 +3674,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="n">
-        <v>3375.806396484375</v>
+        <v>3397.8427734375</v>
       </c>
       <c r="C295" t="n">
         <v>3719.340087890625</v>
@@ -3685,7 +3685,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>3394.341552734375</v>
+        <v>3406.787841796875</v>
       </c>
       <c r="C296" t="n">
         <v>3718.550048828125</v>
@@ -3696,7 +3696,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>3402.569091796875</v>
+        <v>3408.884521484375</v>
       </c>
       <c r="C297" t="n">
         <v>3677.360107421875</v>
@@ -3707,7 +3707,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>3398.145263671875</v>
+        <v>3396.5576171875</v>
       </c>
       <c r="C298" t="n">
         <v>3681.68017578125</v>
@@ -3718,7 +3718,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>3392.733642578125</v>
+        <v>3390.412109375</v>
       </c>
       <c r="C299" t="n">
         <v>3631.199951171875</v>
@@ -3729,7 +3729,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>3379.552978515625</v>
+        <v>3372.3251953125</v>
       </c>
       <c r="C300" t="n">
         <v>3573.629638671875</v>
@@ -3740,7 +3740,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>3356.97216796875</v>
+        <v>3343.71337890625</v>
       </c>
       <c r="C301" t="n">
         <v>3549.590087890625</v>
@@ -3751,7 +3751,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>3333.835693359375</v>
+        <v>3320.70068359375</v>
       </c>
       <c r="C302" t="n">
         <v>3573.18994140625</v>
@@ -3762,7 +3762,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>3322.8681640625</v>
+        <v>3317.7900390625</v>
       </c>
       <c r="C303" t="n">
         <v>3585.199951171875</v>
@@ -3773,7 +3773,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>3321.555908203125</v>
+        <v>3322.49658203125</v>
       </c>
       <c r="C304" t="n">
         <v>3638.030029296875</v>
@@ -3784,7 +3784,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>3333.89501953125</v>
+        <v>3342.511474609375</v>
       </c>
       <c r="C305" t="n">
         <v>3656.6396484375</v>
@@ -3795,7 +3795,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>3349.375732421875</v>
+        <v>3359.737060546875</v>
       </c>
       <c r="C306" t="n">
         <v>3699.820068359375</v>
@@ -3806,7 +3806,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>3368.76025390625</v>
+        <v>3381.326171875</v>
       </c>
       <c r="C307" t="n">
         <v>3626.389892578125</v>
@@ -3817,7 +3817,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="n">
-        <v>3368.409423828125</v>
+        <v>3369.09033203125</v>
       </c>
       <c r="C308" t="n">
         <v>3630.320068359375</v>
@@ -3828,7 +3828,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="n">
-        <v>3363.135986328125</v>
+        <v>3360.615478515625</v>
       </c>
       <c r="C309" t="n">
         <v>3599.919921875</v>
@@ -3839,7 +3839,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>3352.572265625</v>
+        <v>3347.41552734375</v>
       </c>
       <c r="C310" t="n">
         <v>3327.590087890625</v>
@@ -3850,7 +3850,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>3288.40087890625</v>
+        <v>3250.72802734375</v>
       </c>
       <c r="C311" t="n">
         <v>3331.47998046875</v>
@@ -3861,7 +3861,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>3226.579833984375</v>
+        <v>3193.412841796875</v>
       </c>
       <c r="C312" t="n">
         <v>3366.239990234375</v>
@@ -3872,7 +3872,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>3194.598388671875</v>
+        <v>3182.142822265625</v>
       </c>
       <c r="C313" t="n">
         <v>3354.719970703125</v>
@@ -3883,7 +3883,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>3180.0595703125</v>
+        <v>3177.7294921875</v>
       </c>
       <c r="C314" t="n">
         <v>3375.989990234375</v>
@@ -3894,7 +3894,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>3179.47509765625</v>
+        <v>3183.195556640625</v>
       </c>
       <c r="C315" t="n">
         <v>3344.93994140625</v>
@@ -3905,7 +3905,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>3174.77734375</v>
+        <v>3175.995361328125</v>
       </c>
       <c r="C316" t="n">
         <v>3341.8701171875</v>
@@ -3916,7 +3916,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="n">
-        <v>3169.038330078125</v>
+        <v>3169.81787109375</v>
       </c>
       <c r="C317" t="n">
         <v>3320.679931640625</v>
@@ -3927,7 +3927,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="n">
-        <v>3159.77294921875</v>
+        <v>3159.517822265625</v>
       </c>
       <c r="C318" t="n">
         <v>3292.110107421875</v>
@@ -3938,7 +3938,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="n">
-        <v>3145.760009765625</v>
+        <v>3143.890380859375</v>
       </c>
       <c r="C319" t="n">
         <v>3303.5</v>
@@ -3949,7 +3949,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>3137.950439453125</v>
+        <v>3139.5380859375</v>
       </c>
       <c r="C320" t="n">
         <v>3293.969970703125</v>
@@ -3960,7 +3960,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>3132.402587890625</v>
+        <v>3135.317138671875</v>
       </c>
       <c r="C321" t="n">
         <v>3298.989990234375</v>
@@ -3971,7 +3971,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="n">
-        <v>3130.46435546875</v>
+        <v>3134.92138671875</v>
       </c>
       <c r="C322" t="n">
         <v>3241.9599609375</v>
@@ -3982,7 +3982,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="n">
-        <v>3116.0830078125</v>
+        <v>3114.826904296875</v>
       </c>
       <c r="C323" t="n">
         <v>3201.219970703125</v>
@@ -3993,7 +3993,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>3092.75390625</v>
+        <v>3087.840576171875</v>
       </c>
       <c r="C324" t="n">
         <v>3187.75</v>
@@ -4004,7 +4004,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>3071.655029296875</v>
+        <v>3068.751953125</v>
       </c>
       <c r="C325" t="n">
         <v>3199.949951171875</v>
@@ -4015,7 +4015,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>3061.9638671875</v>
+        <v>3064.634033203125</v>
       </c>
       <c r="C326" t="n">
         <v>3265.8701171875</v>
@@ -4026,7 +4026,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>3075.890625</v>
+        <v>3088.130615234375</v>
       </c>
       <c r="C327" t="n">
         <v>3305.780029296875</v>
@@ -4037,7 +4037,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>3100.9423828125</v>
+        <v>3117.0068359375</v>
       </c>
       <c r="C328" t="n">
         <v>3299.179931640625</v>
@@ -4048,7 +4048,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>3117.51318359375</v>
+        <v>3129.26171875</v>
       </c>
       <c r="C329" t="n">
         <v>3316</v>
@@ -4059,7 +4059,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>3129.6201171875</v>
+        <v>3139.3251953125</v>
       </c>
       <c r="C330" t="n">
         <v>3349.6298828125</v>
@@ -4070,7 +4070,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>3144.54443359375</v>
+        <v>3156.005615234375</v>
       </c>
       <c r="C331" t="n">
         <v>3421.570068359375</v>
@@ -4081,7 +4081,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>3172.38134765625</v>
+        <v>3190.0478515625</v>
       </c>
       <c r="C332" t="n">
         <v>3470.7900390625</v>
@@ -4092,7 +4092,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>3205.31396484375</v>
+        <v>3225.43896484375</v>
       </c>
       <c r="C333" t="n">
         <v>3479.000244140625</v>
@@ -4103,7 +4103,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>3229.685791015625</v>
+        <v>3245.5361328125</v>
       </c>
       <c r="C334" t="n">
         <v>3463.1201171875</v>
@@ -4114,7 +4114,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="n">
-        <v>3239.79052734375</v>
+        <v>3248.345458984375</v>
       </c>
       <c r="C335" t="n">
         <v>3478.050048828125</v>
@@ -4125,7 +4125,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>3246.120849609375</v>
+        <v>3252.958984375</v>
       </c>
       <c r="C336" t="n">
         <v>3509.2900390625</v>
@@ -4136,7 +4136,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="n">
-        <v>3256.653076171875</v>
+        <v>3266.06787109375</v>
       </c>
       <c r="C337" t="n">
         <v>3525.499755859375</v>
@@ -4147,7 +4147,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="n">
-        <v>3268.6806640625</v>
+        <v>3278.872314453125</v>
       </c>
       <c r="C338" t="n">
         <v>3484.159912109375</v>
@@ -4158,7 +4158,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="n">
-        <v>3268.2451171875</v>
+        <v>3271.339111328125</v>
       </c>
       <c r="C339" t="n">
         <v>3469.14990234375</v>
@@ -4169,7 +4169,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="n">
-        <v>3261.149169921875</v>
+        <v>3260.337646484375</v>
       </c>
       <c r="C340" t="n">
         <v>3457.169921875</v>
@@ -4180,7 +4180,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="n">
-        <v>3252.174072265625</v>
+        <v>3250.661865234375</v>
       </c>
       <c r="C341" t="n">
         <v>3449.999755859375</v>
@@ -4191,7 +4191,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="n">
-        <v>3244.311279296875</v>
+        <v>3243.70849609375</v>
       </c>
       <c r="C342" t="n">
         <v>3475.7900390625</v>
@@ -4202,7 +4202,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="n">
-        <v>3245.199951171875</v>
+        <v>3249.275634765625</v>
       </c>
       <c r="C343" t="n">
         <v>3488.240234375</v>
@@ -4213,7 +4213,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="n">
-        <v>3251.033447265625</v>
+        <v>3257.56298828125</v>
       </c>
       <c r="C344" t="n">
         <v>3462.519775390625</v>
@@ -4224,7 +4224,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>3250.41015625</v>
+        <v>3253.213134765625</v>
       </c>
       <c r="C345" t="n">
         <v>3355.72998046875</v>
@@ -4235,7 +4235,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>3224.266357421875</v>
+        <v>3213.36962890625</v>
       </c>
       <c r="C346" t="n">
         <v>3343.6298828125</v>
@@ -4246,7 +4246,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="n">
-        <v>3196.248291015625</v>
+        <v>3185.33935546875</v>
       </c>
       <c r="C347" t="n">
         <v>3380.050048828125</v>
@@ -4257,7 +4257,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="n">
-        <v>3186.066162109375</v>
+        <v>3185.682861328125</v>
       </c>
       <c r="C348" t="n">
         <v>3416</v>
@@ -4268,7 +4268,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="n">
-        <v>3193.152587890625</v>
+        <v>3201.4619140625</v>
       </c>
       <c r="C349" t="n">
         <v>3425.52001953125</v>
@@ -4279,7 +4279,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="n">
-        <v>3204.3408203125</v>
+        <v>3213.942138671875</v>
       </c>
       <c r="C350" t="n">
         <v>3405.800048828125</v>
@@ -4290,7 +4290,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>3207.673583984375</v>
+        <v>3212.774658203125</v>
       </c>
       <c r="C351" t="n">
         <v>3315.9599609375</v>
@@ -4301,7 +4301,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="n">
-        <v>3186.736328125</v>
+        <v>3179.662841796875</v>
       </c>
       <c r="C352" t="n">
         <v>3301.1201171875</v>
@@ -4312,7 +4312,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="n">
-        <v>3162.213623046875</v>
+        <v>3154.403076171875</v>
       </c>
       <c r="C353" t="n">
         <v>3285.0400390625</v>
@@ -4323,7 +4323,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>3141.66259765625</v>
+        <v>3137.312255859375</v>
       </c>
       <c r="C354" t="n">
         <v>3283.260009765625</v>
@@ -4334,7 +4334,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="n">
-        <v>3129.087646484375</v>
+        <v>3129.107666015625</v>
       </c>
       <c r="C355" t="n">
         <v>3189.780029296875</v>
@@ -4345,7 +4345,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="n">
-        <v>3099.963623046875</v>
+        <v>3092.46484375</v>
       </c>
       <c r="C356" t="n">
         <v>3221</v>
@@ -4356,7 +4356,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="n">
-        <v>3083.405029296875</v>
+        <v>3081.97216796875</v>
       </c>
       <c r="C357" t="n">
         <v>3262.010009765625</v>
@@ -4367,7 +4367,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="n">
-        <v>3086.990966796875</v>
+        <v>3094.729248046875</v>
       </c>
       <c r="C358" t="n">
         <v>3302.429931640625</v>
@@ -4378,7 +4378,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>3104.754638671875</v>
+        <v>3118.00439453125</v>
       </c>
       <c r="C359" t="n">
         <v>3288.6201171875</v>
@@ -4389,7 +4389,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="n">
-        <v>3115.857177734375</v>
+        <v>3125.51708984375</v>
       </c>
       <c r="C360" t="n">
         <v>3246.300048828125</v>
@@ -4400,7 +4400,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="n">
-        <v>3110.219970703125</v>
+        <v>3112.251953125</v>
       </c>
       <c r="C361" t="n">
         <v>3247.330078125</v>
@@ -4411,7 +4411,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>3102.130859375</v>
+        <v>3103.734375</v>
       </c>
       <c r="C362" t="n">
         <v>3284.280029296875</v>
@@ -4422,7 +4422,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="n">
-        <v>3105.86083984375</v>
+        <v>3113.455078125</v>
       </c>
       <c r="C363" t="n">
         <v>3299.860107421875</v>
@@ -4433,7 +4433,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="n">
-        <v>3115.6533203125</v>
+        <v>3125.89990234375</v>
       </c>
       <c r="C364" t="n">
         <v>3409.02001953125</v>
@@ -4444,7 +4444,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>3150.118896484375</v>
+        <v>3170.568603515625</v>
       </c>
       <c r="C365" t="n">
         <v>3446.739990234375</v>
@@ -4455,7 +4455,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="n">
-        <v>3187.40185546875</v>
+        <v>3208.902587890625</v>
       </c>
       <c r="C366" t="n">
         <v>3444.14990234375</v>
@@ -4466,7 +4466,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="n">
-        <v>3211.029296875</v>
+        <v>3225.862060546875</v>
       </c>
       <c r="C367" t="n">
         <v>3415.06005859375</v>
@@ -4477,7 +4477,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>3216.139892578125</v>
+        <v>3221.947998046875</v>
       </c>
       <c r="C368" t="n">
         <v>3435.010009765625</v>
@@ -4488,7 +4488,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>3219.25439453125</v>
+        <v>3224.6689453125</v>
       </c>
       <c r="C369" t="n">
         <v>3335.550048828125</v>
@@ -4499,7 +4499,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>3198.86474609375</v>
+        <v>3192.910400390625</v>
       </c>
       <c r="C370" t="n">
         <v>3320.3701171875</v>
@@ -4510,7 +4510,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>3175.0126953125</v>
+        <v>3167.874267578125</v>
       </c>
       <c r="C371" t="n">
         <v>3376.070068359375</v>
@@ -4521,7 +4521,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>3171.9521484375</v>
+        <v>3175.84765625</v>
       </c>
       <c r="C372" t="n">
         <v>3392.489990234375</v>
@@ -4532,7 +4532,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>3180.10205078125</v>
+        <v>3189.244384765625</v>
       </c>
       <c r="C373" t="n">
         <v>3446.570068359375</v>
@@ -4543,7 +4543,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>3200.60888671875</v>
+        <v>3214.744873046875</v>
       </c>
       <c r="C374" t="n">
         <v>3372.429931640625</v>
@@ -4554,7 +4554,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>3199.8974609375</v>
+        <v>3203.098388671875</v>
       </c>
       <c r="C375" t="n">
         <v>3318.110107421875</v>
@@ -4565,7 +4565,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>3180.478515625</v>
+        <v>3174.255859375</v>
       </c>
       <c r="C376" t="n">
         <v>3312.75</v>
@@ -4576,7 +4576,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>3161.184326171875</v>
+        <v>3156.281494140625</v>
       </c>
       <c r="C377" t="n">
         <v>3384</v>
@@ -4587,7 +4587,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>3166.051513671875</v>
+        <v>3173.721923828125</v>
       </c>
       <c r="C378" t="n">
         <v>3477</v>
@@ -4598,7 +4598,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>3198.06201171875</v>
+        <v>3218.224609375</v>
       </c>
       <c r="C379" t="n">
         <v>3518.989990234375</v>
@@ -4609,7 +4609,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>3234.914794921875</v>
+        <v>3256.729736328125</v>
       </c>
       <c r="C380" t="n">
         <v>3488.97998046875</v>
@@ -4620,7 +4620,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>3252.77197265625</v>
+        <v>3264.556396484375</v>
       </c>
       <c r="C381" t="n">
         <v>3576.22998046875</v>
@@ -4631,7 +4631,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>3278.105224609375</v>
+        <v>3293.92529296875</v>
       </c>
       <c r="C382" t="n">
         <v>3482.050048828125</v>
@@ -4642,7 +4642,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>3277.330078125</v>
+        <v>3279.837158203125</v>
       </c>
       <c r="C383" t="n">
         <v>3472.500244140625</v>
@@ -4653,7 +4653,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>3267.382080078125</v>
+        <v>3264.82666015625</v>
       </c>
       <c r="C384" t="n">
         <v>3525.14990234375</v>
@@ -4664,7 +4664,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>3270.113525390625</v>
+        <v>3275.137939453125</v>
       </c>
       <c r="C385" t="n">
         <v>3545.6796875</v>
@@ -4675,7 +4675,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>3280.53515625</v>
+        <v>3289.930908203125</v>
       </c>
       <c r="C386" t="n">
         <v>3540.699951171875</v>
@@ -4686,7 +4686,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>3288.42431640625</v>
+        <v>3295.844970703125</v>
       </c>
       <c r="C387" t="n">
         <v>3549</v>
@@ -4697,7 +4697,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>3294.510986328125</v>
+        <v>3300.391845703125</v>
       </c>
       <c r="C388" t="n">
         <v>3696.06005859375</v>
@@ -4708,7 +4708,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>3328.7158203125</v>
+        <v>3350.0966796875</v>
       </c>
       <c r="C389" t="n">
         <v>3676.570068359375</v>
@@ -4719,7 +4719,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>3355.17431640625</v>
+        <v>3372.816650390625</v>
       </c>
       <c r="C390" t="n">
         <v>3572.56982421875</v>
@@ -4730,7 +4730,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>3349.689697265625</v>
+        <v>3347.56591796875</v>
       </c>
       <c r="C391" t="n">
         <v>3580.0400390625</v>
@@ -4741,7 +4741,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>3338.22998046875</v>
+        <v>3332.3046875</v>
       </c>
       <c r="C392" t="n">
         <v>3580.41015625</v>
@@ -4752,7 +4752,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>3329.6064453125</v>
+        <v>3326.497802734375</v>
       </c>
       <c r="C393" t="n">
         <v>3504.559814453125</v>
@@ -4763,7 +4763,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>3309.44873046875</v>
+        <v>3300.014892578125</v>
       </c>
       <c r="C394" t="n">
         <v>3561.570068359375</v>
@@ -4800,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>179.9438280408639</v>
+        <v>173.2912277334747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>